<commit_message>
all source and test
</commit_message>
<xml_diff>
--- a/BaoCao_SystemTest_AdminOrder.xlsx
+++ b/BaoCao_SystemTest_AdminOrder.xlsx
@@ -42,17 +42,17 @@
   </si>
   <si>
     <t>1. Vào Menu -&gt; iframe
-2. Click nút 'Chi tiết' (Mắt)
-3. Check trang chi tiết</t>
+2. Click nút 'Chi tiết' (Mắt) đơn đầu tiên
+3. Kiểm tra nội dung trang</t>
   </si>
   <si>
     <t>Click icon 👁️</t>
   </si>
   <si>
-    <t>Chuyển trang &amp; Hiển thị đúng thông tin</t>
-  </si>
-  <si>
-    <t>Tiêu đề: 📦 Chi tiết đơn hàng #122</t>
+    <t>Chuyển trang thành công, tiêu đề chứa Order ID và Bảng chi tiết sản phẩm không trống</t>
+  </si>
+  <si>
+    <t>Tiêu đề: 📦 Chi tiết đơn hàng #2067</t>
   </si>
   <si>
     <t>PASS</t>
@@ -65,14 +65,14 @@
   </si>
   <si>
     <t>1. Vào Menu -&gt; iframe
-2. Chọn đơn đầu tiên
-3. Đổi sang 'Đang giao hàng'</t>
+2. Chọn dropdown đơn đầu tiên
+3. Đổi trạng thái sang 'Đang giao hàng'</t>
   </si>
   <si>
     <t>Status: Đang giao hàng</t>
   </si>
   <si>
-    <t>Trạng thái được cập nhật thành công</t>
+    <t>Trạng thái được cập nhật thành công và hiển thị 'Đang giao hàng'</t>
   </si>
   <si>
     <t>Trạng thái mới: Đang giao hàng</t>
@@ -86,7 +86,7 @@
   <si>
     <t>1. Click Menu 'Quản lý hóa đơn'
 2. Chuyển vào iframe
-3. Lọc 'Chờ xử lý'</t>
+3. Chọn và Lọc 'Chờ xử lý'</t>
   </si>
   <si>
     <t>Filter: Chờ xử lý</t>
@@ -181,10 +181,10 @@
   <cols>
     <col min="1" max="1" width="21.39453125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="27.25390625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="29.421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="36.2890625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="21.44921875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="46.75390625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="30.75" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="78.69140625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="31.86328125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="10.62890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>